<commit_message>
Fix a mismatched master_code
</commit_message>
<xml_diff>
--- a/tests/files/invoices/order_sheet_invoice_simple.xlsx
+++ b/tests/files/invoices/order_sheet_invoice_simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="262">
   <si>
     <t>주문고유번호</t>
   </si>
@@ -226,9 +226,6 @@
     <t>509255530766</t>
   </si>
   <si>
-    <t>OPT30</t>
-  </si>
-  <si>
     <t>100044781917</t>
   </si>
   <si>
@@ -268,259 +265,259 @@
     <t>509255530770</t>
   </si>
   <si>
+    <t>101386327356</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 12:09:00</t>
+  </si>
+  <si>
+    <t>2722443742</t>
+  </si>
+  <si>
+    <t>hwangsj91</t>
+  </si>
+  <si>
+    <t>황승주</t>
+  </si>
+  <si>
+    <t>010-5161-2122</t>
+  </si>
+  <si>
+    <t>42995</t>
+  </si>
+  <si>
+    <t>대구광역시 달성군 현풍읍 테크노북로4길 27  (대구테크노폴리스엘에이치천년나무3단지) 302/1611</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2722443742)</t>
+  </si>
+  <si>
+    <t>509255530781</t>
+  </si>
+  <si>
+    <t>100654349913</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 10:13:00</t>
+  </si>
+  <si>
+    <t>2722218050</t>
+  </si>
+  <si>
+    <t>2892531758</t>
+  </si>
+  <si>
+    <t>[템테이션] 고양이 간식 5개 세트 모음전</t>
+  </si>
+  <si>
+    <t>풍부한 해산물맛 85gx5개</t>
+  </si>
+  <si>
+    <t>riverhee314</t>
+  </si>
+  <si>
+    <t>김혜진</t>
+  </si>
+  <si>
+    <t>010-9697-1223</t>
+  </si>
+  <si>
+    <t>61075</t>
+  </si>
+  <si>
+    <t>광주광역시 북구 효열로 11  (연제동) 광명2차 201동1102호</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2722218050)</t>
+  </si>
+  <si>
+    <t>509255530814</t>
+  </si>
+  <si>
+    <t>set3x5</t>
+  </si>
+  <si>
+    <t>헤어볼컨트롤 60gx5개</t>
+  </si>
+  <si>
+    <t>set4x5</t>
+  </si>
+  <si>
+    <t>101136042848</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:10</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 12:54:00</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:19</t>
+  </si>
+  <si>
+    <t>2721607570</t>
+  </si>
+  <si>
+    <t>4022668750</t>
+  </si>
+  <si>
+    <t>[애견용품] 탈취제세정제물티슈샴푸배변유도제보습제치약</t>
+  </si>
+  <si>
+    <t>07.[에티펫] 손발 엉덩이 깨끗 아쿠아물티슈80매</t>
+  </si>
+  <si>
+    <t>rlaguswn1109</t>
+  </si>
+  <si>
+    <t>김태겸</t>
+  </si>
+  <si>
+    <t>010-2349-0418</t>
+  </si>
+  <si>
+    <t>김푸른</t>
+  </si>
+  <si>
+    <t>11689</t>
+  </si>
+  <si>
+    <t>경기도 의정부시 호국로1297번길 8-3  (의정부동) 3층</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2721607570)</t>
+  </si>
+  <si>
+    <t>509255530943</t>
+  </si>
+  <si>
+    <t>103948571494</t>
+  </si>
+  <si>
+    <t>고도몰5</t>
+  </si>
+  <si>
+    <t>B691</t>
+  </si>
+  <si>
+    <t>esc0711</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:06</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 10:14:14</t>
+  </si>
+  <si>
+    <t>2010052213352735 395185</t>
+  </si>
+  <si>
+    <t>1000014019</t>
+  </si>
+  <si>
+    <t>[웰컴템-100원] 굿프랜드 고양이캔 (참치&amp;새우) 85g x5개</t>
+  </si>
+  <si>
+    <t>추가구매상품 없음</t>
+  </si>
+  <si>
+    <t>조민지</t>
+  </si>
+  <si>
+    <t>010-4108-8464</t>
+  </si>
+  <si>
+    <t>10516</t>
+  </si>
+  <si>
+    <t>경기도 고양시 덕양구 행당로 34-20 (벽산아파트) 101동 109호</t>
+  </si>
+  <si>
+    <t>509255531116</t>
+  </si>
+  <si>
+    <t>COM2</t>
+  </si>
+  <si>
+    <t>102527600530</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:05</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 9:19:43</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:20</t>
+  </si>
+  <si>
+    <t>2010052117060776 395150</t>
+  </si>
+  <si>
+    <t>1000014009</t>
+  </si>
+  <si>
+    <t>[웰컴템-100원] 더캣츠 베로베로젤 닭&amp;참치 10gx20p</t>
+  </si>
+  <si>
+    <t>김효정</t>
+  </si>
+  <si>
+    <t>010-2792-5596</t>
+  </si>
+  <si>
+    <t>16959</t>
+  </si>
+  <si>
+    <t>경기도 용인시 기흥구 기흥로116번길 5 (새릉골풍림아파트) 102동 1702호</t>
+  </si>
+  <si>
+    <t>509255531201</t>
+  </si>
+  <si>
+    <t>COM4</t>
+  </si>
+  <si>
+    <t>100056849185</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:00</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 3:57:20</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:21</t>
+  </si>
+  <si>
+    <t>2010051556318808 394930</t>
+  </si>
+  <si>
+    <t>1000012362</t>
+  </si>
+  <si>
+    <t>앤디와 친구들 라텍스 토이</t>
+  </si>
+  <si>
+    <t>선택:데이지(닭)</t>
+  </si>
+  <si>
+    <t>이서윤</t>
+  </si>
+  <si>
+    <t>010-4224-1908</t>
+  </si>
+  <si>
+    <t>05501</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 올림픽로 99 (잠실엘스) 132-2304</t>
+  </si>
+  <si>
+    <t>509255531503</t>
+  </si>
+  <si>
     <t>OPT8</t>
-  </si>
-  <si>
-    <t>101386327356</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 12:09:00</t>
-  </si>
-  <si>
-    <t>2722443742</t>
-  </si>
-  <si>
-    <t>hwangsj91</t>
-  </si>
-  <si>
-    <t>황승주</t>
-  </si>
-  <si>
-    <t>010-5161-2122</t>
-  </si>
-  <si>
-    <t>42995</t>
-  </si>
-  <si>
-    <t>대구광역시 달성군 현풍읍 테크노북로4길 27  (대구테크노폴리스엘에이치천년나무3단지) 302/1611</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2722443742)</t>
-  </si>
-  <si>
-    <t>509255530781</t>
-  </si>
-  <si>
-    <t>100654349913</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 10:13:00</t>
-  </si>
-  <si>
-    <t>2722218050</t>
-  </si>
-  <si>
-    <t>2892531758</t>
-  </si>
-  <si>
-    <t>[템테이션] 고양이 간식 5개 세트 모음전</t>
-  </si>
-  <si>
-    <t>풍부한 해산물맛 85gx5개</t>
-  </si>
-  <si>
-    <t>riverhee314</t>
-  </si>
-  <si>
-    <t>김혜진</t>
-  </si>
-  <si>
-    <t>010-9697-1223</t>
-  </si>
-  <si>
-    <t>61075</t>
-  </si>
-  <si>
-    <t>광주광역시 북구 효열로 11  (연제동) 광명2차 201동1102호</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2722218050)</t>
-  </si>
-  <si>
-    <t>509255530814</t>
-  </si>
-  <si>
-    <t>set3x5</t>
-  </si>
-  <si>
-    <t>헤어볼컨트롤 60gx5개</t>
-  </si>
-  <si>
-    <t>set4x5</t>
-  </si>
-  <si>
-    <t>101136042848</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:10</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 12:54:00</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:19</t>
-  </si>
-  <si>
-    <t>2721607570</t>
-  </si>
-  <si>
-    <t>4022668750</t>
-  </si>
-  <si>
-    <t>[애견용품] 탈취제세정제물티슈샴푸배변유도제보습제치약</t>
-  </si>
-  <si>
-    <t>07.[에티펫] 손발 엉덩이 깨끗 아쿠아물티슈80매</t>
-  </si>
-  <si>
-    <t>rlaguswn1109</t>
-  </si>
-  <si>
-    <t>김태겸</t>
-  </si>
-  <si>
-    <t>010-2349-0418</t>
-  </si>
-  <si>
-    <t>김푸른</t>
-  </si>
-  <si>
-    <t>11689</t>
-  </si>
-  <si>
-    <t>경기도 의정부시 호국로1297번길 8-3  (의정부동) 3층</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2721607570)</t>
-  </si>
-  <si>
-    <t>509255530943</t>
-  </si>
-  <si>
-    <t>103948571494</t>
-  </si>
-  <si>
-    <t>고도몰5</t>
-  </si>
-  <si>
-    <t>B691</t>
-  </si>
-  <si>
-    <t>esc0711</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:06</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 10:14:14</t>
-  </si>
-  <si>
-    <t>2010052213352735 395185</t>
-  </si>
-  <si>
-    <t>1000014019</t>
-  </si>
-  <si>
-    <t>[웰컴템-100원] 굿프랜드 고양이캔 (참치&amp;새우) 85g x5개</t>
-  </si>
-  <si>
-    <t>추가구매상품 없음</t>
-  </si>
-  <si>
-    <t>조민지</t>
-  </si>
-  <si>
-    <t>010-4108-8464</t>
-  </si>
-  <si>
-    <t>10516</t>
-  </si>
-  <si>
-    <t>경기도 고양시 덕양구 행당로 34-20 (벽산아파트) 101동 109호</t>
-  </si>
-  <si>
-    <t>509255531116</t>
-  </si>
-  <si>
-    <t>COM2</t>
-  </si>
-  <si>
-    <t>102527600530</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:05</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 9:19:43</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:20</t>
-  </si>
-  <si>
-    <t>2010052117060776 395150</t>
-  </si>
-  <si>
-    <t>1000014009</t>
-  </si>
-  <si>
-    <t>[웰컴템-100원] 더캣츠 베로베로젤 닭&amp;참치 10gx20p</t>
-  </si>
-  <si>
-    <t>김효정</t>
-  </si>
-  <si>
-    <t>010-2792-5596</t>
-  </si>
-  <si>
-    <t>16959</t>
-  </si>
-  <si>
-    <t>경기도 용인시 기흥구 기흥로116번길 5 (새릉골풍림아파트) 102동 1702호</t>
-  </si>
-  <si>
-    <t>509255531201</t>
-  </si>
-  <si>
-    <t>COM4</t>
-  </si>
-  <si>
-    <t>100056849185</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:00</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 3:57:20</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:21</t>
-  </si>
-  <si>
-    <t>2010051556318808 394930</t>
-  </si>
-  <si>
-    <t>1000012362</t>
-  </si>
-  <si>
-    <t>앤디와 친구들 라텍스 토이</t>
-  </si>
-  <si>
-    <t>선택:데이지(닭)</t>
-  </si>
-  <si>
-    <t>이서윤</t>
-  </si>
-  <si>
-    <t>010-4224-1908</t>
-  </si>
-  <si>
-    <t>05501</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 올림픽로 99 (잠실엘스) 132-2304</t>
-  </si>
-  <si>
-    <t>509255531503</t>
   </si>
   <si>
     <t>103247553909</t>
@@ -877,13 +874,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,17 +1497,17 @@
       <c r="AP2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AQ2" s="4" t="s">
-        <v>70</v>
+      <c r="AQ2" s="4">
+        <v>7</v>
       </c>
       <c r="AR2" s="3"/>
-      <c r="AS2" s="4" t="s">
-        <v>70</v>
+      <c r="AS2" s="4">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>46</v>
@@ -1528,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>52</v>
@@ -1543,17 +1540,17 @@
         <v>54</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>59</v>
@@ -1596,52 +1593,52 @@
         <v>0</v>
       </c>
       <c r="AE3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AH3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="AO3" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>1</v>
       </c>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="4" t="s">
-        <v>84</v>
+      <c r="AS3" s="4">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>46</v>
@@ -1659,10 +1656,10 @@
         <v>50</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>52</v>
@@ -1674,17 +1671,17 @@
         <v>54</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>59</v>
@@ -1727,40 +1724,40 @@
         <v>0</v>
       </c>
       <c r="AE4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AH4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="AO4" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AQ4" s="4">
         <v>2</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>46</v>
@@ -1790,10 +1787,10 @@
         <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>52</v>
@@ -1805,17 +1802,17 @@
         <v>54</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>59</v>
@@ -1858,52 +1855,52 @@
         <v>0</v>
       </c>
       <c r="AE5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AM5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AH5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL5" s="3" t="s">
+      <c r="AN5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="AM5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN5" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="AO5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AR5" s="3"/>
       <c r="AS5" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>46</v>
@@ -1921,10 +1918,10 @@
         <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>52</v>
@@ -1936,17 +1933,17 @@
         <v>54</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>59</v>
@@ -1989,52 +1986,52 @@
         <v>0</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AM6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AN6" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="AM6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN6" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="AO6" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AR6" s="3"/>
       <c r="AS6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
@@ -2049,16 +2046,16 @@
         <v>49</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>53</v>
@@ -2067,17 +2064,17 @@
         <v>54</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>59</v>
@@ -2120,40 +2117,40 @@
         <v>0</v>
       </c>
       <c r="AE7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AF7" s="3" t="s">
+      <c r="AH7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI7" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AG7" s="3" t="s">
+      <c r="AJ7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL7" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AH7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI7" s="3" t="s">
+      <c r="AM7" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AJ7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL7" s="3" t="s">
+      <c r="AN7" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="AM7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AN7" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="AO7" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AQ7" s="4">
         <v>3</v>
@@ -2165,31 +2162,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>53</v>
@@ -2198,13 +2195,13 @@
         <v>54</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -2212,7 +2209,7 @@
         <v>59</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>59</v>
@@ -2252,69 +2249,69 @@
       </c>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM8" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="AI8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM8" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="AN8" s="3"/>
       <c r="AO8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AQ8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AR8" s="3"/>
       <c r="AS8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>53</v>
@@ -2323,13 +2320,13 @@
         <v>54</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -2337,7 +2334,7 @@
         <v>59</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>59</v>
@@ -2377,67 +2374,67 @@
       </c>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM9" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="AL9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AM9" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="AN9" s="3"/>
       <c r="AO9" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP9" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AQ9" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AR9" s="3"/>
       <c r="AS9" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>53</v>
@@ -2446,23 +2443,23 @@
         <v>54</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>59</v>
@@ -2502,67 +2499,67 @@
       </c>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AI10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM10" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="AL10" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM10" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="AN10" s="3"/>
       <c r="AO10" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP10" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AQ10" s="5" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="AR10" s="3"/>
       <c r="AS10" s="5" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>53</v>
@@ -2571,13 +2568,13 @@
         <v>54</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -2623,55 +2620,55 @@
       </c>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG11" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AG11" s="3" t="s">
+      <c r="AH11" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AH11" s="3" t="s">
+      <c r="AK11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AI11" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
+      <c r="AL11" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AK11" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL11" s="3" t="s">
+      <c r="AM11" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AM11" s="3" t="s">
+      <c r="AN11" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="AN11" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="AO11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP11" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ11" s="4">
         <v>8</v>
       </c>
       <c r="AR11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AS11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>48</v>
@@ -2680,16 +2677,16 @@
         <v>49</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>53</v>
@@ -2698,13 +2695,13 @@
         <v>54</v>
       </c>
       <c r="L12" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -2734,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="Z12" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB12" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="AC12" s="4">
         <v>0</v>
@@ -2750,67 +2747,67 @@
       </c>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG12" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="AG12" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM12" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="AM12" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="AN12" s="3"/>
       <c r="AO12" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ12" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="AQ12" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="AR12" s="3"/>
       <c r="AS12" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>53</v>
@@ -2819,17 +2816,17 @@
         <v>54</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>59</v>
@@ -2857,13 +2854,13 @@
         <v>1</v>
       </c>
       <c r="Z13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB13" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="AC13" s="4">
         <v>0</v>
@@ -2873,67 +2870,67 @@
       </c>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AJ13" s="3" t="s">
+      <c r="AK13" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AL13" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AK13" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AL13" s="3" t="s">
+      <c r="AM13" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="AM13" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="AN13" s="3"/>
       <c r="AO13" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP13" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AQ13" s="4">
         <v>9</v>
       </c>
       <c r="AR13" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AS13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>53</v>
@@ -2942,13 +2939,13 @@
         <v>54</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2994,35 +2991,35 @@
       </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG14" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AG14" s="3" t="s">
+      <c r="AH14" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="AH14" s="3" t="s">
+      <c r="AI14" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="AI14" s="3" t="s">
+      <c r="AJ14" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="AJ14" s="3" t="s">
+      <c r="AK14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL14" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="AK14" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="AL14" s="3" t="s">
+      <c r="AM14" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="AM14" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="AN14" s="3"/>
       <c r="AO14" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP14" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AQ14" s="4">
         <v>4</v>
@@ -3032,31 +3029,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>53</v>
@@ -3065,17 +3062,17 @@
         <v>54</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>59</v>
@@ -3103,14 +3100,14 @@
         <v>1</v>
       </c>
       <c r="Z15" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB15" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AA15" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="AC15" s="4">
         <v>0</v>
       </c>
@@ -3118,47 +3115,47 @@
         <v>0</v>
       </c>
       <c r="AE15" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF15" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="AF15" s="3" t="s">
+      <c r="AG15" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="AG15" s="3" t="s">
+      <c r="AH15" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AH15" s="3" t="s">
+      <c r="AI15" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL15" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="AI15" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AK15" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AL15" s="3" t="s">
+      <c r="AM15" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AM15" s="3" t="s">
+      <c r="AN15" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="AN15" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="AO15" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP15" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AQ15" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="AQ15" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="AR15" s="3"/>
       <c r="AS15" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the function with a printing of `Order` table (#46)
* Add CANCEL status to `OrderSheetInvoice` resource

* Create `Upload File Again` action to `OrderShipmentInvoice` resource

* Install `carlos-meneses/laravel-mpdf` package

* Create printing `OrderSheetInvoice`s

* Change `ChangeStatusAction` name() for better visible

* Translate a sentence

* Remove `is_all_good_matched` field in `orders` table

* Set up `Order` model related processes

* Fix a mismatched master_code

* Make a relation between `OrderShipment` and `Order`

* Add `invoice_numbers` field into `order_shipments` table

* Complete the function of `Order` printing
</commit_message>
<xml_diff>
--- a/tests/files/invoices/order_sheet_invoice_simple.xlsx
+++ b/tests/files/invoices/order_sheet_invoice_simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="262">
   <si>
     <t>주문고유번호</t>
   </si>
@@ -226,9 +226,6 @@
     <t>509255530766</t>
   </si>
   <si>
-    <t>OPT30</t>
-  </si>
-  <si>
     <t>100044781917</t>
   </si>
   <si>
@@ -268,259 +265,259 @@
     <t>509255530770</t>
   </si>
   <si>
+    <t>101386327356</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 12:09:00</t>
+  </si>
+  <si>
+    <t>2722443742</t>
+  </si>
+  <si>
+    <t>hwangsj91</t>
+  </si>
+  <si>
+    <t>황승주</t>
+  </si>
+  <si>
+    <t>010-5161-2122</t>
+  </si>
+  <si>
+    <t>42995</t>
+  </si>
+  <si>
+    <t>대구광역시 달성군 현풍읍 테크노북로4길 27  (대구테크노폴리스엘에이치천년나무3단지) 302/1611</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2722443742)</t>
+  </si>
+  <si>
+    <t>509255530781</t>
+  </si>
+  <si>
+    <t>100654349913</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 10:13:00</t>
+  </si>
+  <si>
+    <t>2722218050</t>
+  </si>
+  <si>
+    <t>2892531758</t>
+  </si>
+  <si>
+    <t>[템테이션] 고양이 간식 5개 세트 모음전</t>
+  </si>
+  <si>
+    <t>풍부한 해산물맛 85gx5개</t>
+  </si>
+  <si>
+    <t>riverhee314</t>
+  </si>
+  <si>
+    <t>김혜진</t>
+  </si>
+  <si>
+    <t>010-9697-1223</t>
+  </si>
+  <si>
+    <t>61075</t>
+  </si>
+  <si>
+    <t>광주광역시 북구 효열로 11  (연제동) 광명2차 201동1102호</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2722218050)</t>
+  </si>
+  <si>
+    <t>509255530814</t>
+  </si>
+  <si>
+    <t>set3x5</t>
+  </si>
+  <si>
+    <t>헤어볼컨트롤 60gx5개</t>
+  </si>
+  <si>
+    <t>set4x5</t>
+  </si>
+  <si>
+    <t>101136042848</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:10</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 12:54:00</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:19</t>
+  </si>
+  <si>
+    <t>2721607570</t>
+  </si>
+  <si>
+    <t>4022668750</t>
+  </si>
+  <si>
+    <t>[애견용품] 탈취제세정제물티슈샴푸배변유도제보습제치약</t>
+  </si>
+  <si>
+    <t>07.[에티펫] 손발 엉덩이 깨끗 아쿠아물티슈80매</t>
+  </si>
+  <si>
+    <t>rlaguswn1109</t>
+  </si>
+  <si>
+    <t>김태겸</t>
+  </si>
+  <si>
+    <t>010-2349-0418</t>
+  </si>
+  <si>
+    <t>김푸른</t>
+  </si>
+  <si>
+    <t>11689</t>
+  </si>
+  <si>
+    <t>경기도 의정부시 호국로1297번길 8-3  (의정부동) 3층</t>
+  </si>
+  <si>
+    <t>(주문번호 : 2721607570)</t>
+  </si>
+  <si>
+    <t>509255530943</t>
+  </si>
+  <si>
+    <t>103948571494</t>
+  </si>
+  <si>
+    <t>고도몰5</t>
+  </si>
+  <si>
+    <t>B691</t>
+  </si>
+  <si>
+    <t>esc0711</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:06</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 10:14:14</t>
+  </si>
+  <si>
+    <t>2010052213352735 395185</t>
+  </si>
+  <si>
+    <t>1000014019</t>
+  </si>
+  <si>
+    <t>[웰컴템-100원] 굿프랜드 고양이캔 (참치&amp;새우) 85g x5개</t>
+  </si>
+  <si>
+    <t>추가구매상품 없음</t>
+  </si>
+  <si>
+    <t>조민지</t>
+  </si>
+  <si>
+    <t>010-4108-8464</t>
+  </si>
+  <si>
+    <t>10516</t>
+  </si>
+  <si>
+    <t>경기도 고양시 덕양구 행당로 34-20 (벽산아파트) 101동 109호</t>
+  </si>
+  <si>
+    <t>509255531116</t>
+  </si>
+  <si>
+    <t>COM2</t>
+  </si>
+  <si>
+    <t>102527600530</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:05</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 9:19:43</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:20</t>
+  </si>
+  <si>
+    <t>2010052117060776 395150</t>
+  </si>
+  <si>
+    <t>1000014009</t>
+  </si>
+  <si>
+    <t>[웰컴템-100원] 더캣츠 베로베로젤 닭&amp;참치 10gx20p</t>
+  </si>
+  <si>
+    <t>김효정</t>
+  </si>
+  <si>
+    <t>010-2792-5596</t>
+  </si>
+  <si>
+    <t>16959</t>
+  </si>
+  <si>
+    <t>경기도 용인시 기흥구 기흥로116번길 5 (새릉골풍림아파트) 102동 1702호</t>
+  </si>
+  <si>
+    <t>509255531201</t>
+  </si>
+  <si>
+    <t>COM4</t>
+  </si>
+  <si>
+    <t>100056849185</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:03:00</t>
+  </si>
+  <si>
+    <t>2020-10-05 오후 3:57:20</t>
+  </si>
+  <si>
+    <t>2020-10-06 오전 7:29:21</t>
+  </si>
+  <si>
+    <t>2010051556318808 394930</t>
+  </si>
+  <si>
+    <t>1000012362</t>
+  </si>
+  <si>
+    <t>앤디와 친구들 라텍스 토이</t>
+  </si>
+  <si>
+    <t>선택:데이지(닭)</t>
+  </si>
+  <si>
+    <t>이서윤</t>
+  </si>
+  <si>
+    <t>010-4224-1908</t>
+  </si>
+  <si>
+    <t>05501</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 올림픽로 99 (잠실엘스) 132-2304</t>
+  </si>
+  <si>
+    <t>509255531503</t>
+  </si>
+  <si>
     <t>OPT8</t>
-  </si>
-  <si>
-    <t>101386327356</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 12:09:00</t>
-  </si>
-  <si>
-    <t>2722443742</t>
-  </si>
-  <si>
-    <t>hwangsj91</t>
-  </si>
-  <si>
-    <t>황승주</t>
-  </si>
-  <si>
-    <t>010-5161-2122</t>
-  </si>
-  <si>
-    <t>42995</t>
-  </si>
-  <si>
-    <t>대구광역시 달성군 현풍읍 테크노북로4길 27  (대구테크노폴리스엘에이치천년나무3단지) 302/1611</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2722443742)</t>
-  </si>
-  <si>
-    <t>509255530781</t>
-  </si>
-  <si>
-    <t>100654349913</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 10:13:00</t>
-  </si>
-  <si>
-    <t>2722218050</t>
-  </si>
-  <si>
-    <t>2892531758</t>
-  </si>
-  <si>
-    <t>[템테이션] 고양이 간식 5개 세트 모음전</t>
-  </si>
-  <si>
-    <t>풍부한 해산물맛 85gx5개</t>
-  </si>
-  <si>
-    <t>riverhee314</t>
-  </si>
-  <si>
-    <t>김혜진</t>
-  </si>
-  <si>
-    <t>010-9697-1223</t>
-  </si>
-  <si>
-    <t>61075</t>
-  </si>
-  <si>
-    <t>광주광역시 북구 효열로 11  (연제동) 광명2차 201동1102호</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2722218050)</t>
-  </si>
-  <si>
-    <t>509255530814</t>
-  </si>
-  <si>
-    <t>set3x5</t>
-  </si>
-  <si>
-    <t>헤어볼컨트롤 60gx5개</t>
-  </si>
-  <si>
-    <t>set4x5</t>
-  </si>
-  <si>
-    <t>101136042848</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:10</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 12:54:00</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:19</t>
-  </si>
-  <si>
-    <t>2721607570</t>
-  </si>
-  <si>
-    <t>4022668750</t>
-  </si>
-  <si>
-    <t>[애견용품] 탈취제세정제물티슈샴푸배변유도제보습제치약</t>
-  </si>
-  <si>
-    <t>07.[에티펫] 손발 엉덩이 깨끗 아쿠아물티슈80매</t>
-  </si>
-  <si>
-    <t>rlaguswn1109</t>
-  </si>
-  <si>
-    <t>김태겸</t>
-  </si>
-  <si>
-    <t>010-2349-0418</t>
-  </si>
-  <si>
-    <t>김푸른</t>
-  </si>
-  <si>
-    <t>11689</t>
-  </si>
-  <si>
-    <t>경기도 의정부시 호국로1297번길 8-3  (의정부동) 3층</t>
-  </si>
-  <si>
-    <t>(주문번호 : 2721607570)</t>
-  </si>
-  <si>
-    <t>509255530943</t>
-  </si>
-  <si>
-    <t>103948571494</t>
-  </si>
-  <si>
-    <t>고도몰5</t>
-  </si>
-  <si>
-    <t>B691</t>
-  </si>
-  <si>
-    <t>esc0711</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:06</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 10:14:14</t>
-  </si>
-  <si>
-    <t>2010052213352735 395185</t>
-  </si>
-  <si>
-    <t>1000014019</t>
-  </si>
-  <si>
-    <t>[웰컴템-100원] 굿프랜드 고양이캔 (참치&amp;새우) 85g x5개</t>
-  </si>
-  <si>
-    <t>추가구매상품 없음</t>
-  </si>
-  <si>
-    <t>조민지</t>
-  </si>
-  <si>
-    <t>010-4108-8464</t>
-  </si>
-  <si>
-    <t>10516</t>
-  </si>
-  <si>
-    <t>경기도 고양시 덕양구 행당로 34-20 (벽산아파트) 101동 109호</t>
-  </si>
-  <si>
-    <t>509255531116</t>
-  </si>
-  <si>
-    <t>COM2</t>
-  </si>
-  <si>
-    <t>102527600530</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:05</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 9:19:43</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:20</t>
-  </si>
-  <si>
-    <t>2010052117060776 395150</t>
-  </si>
-  <si>
-    <t>1000014009</t>
-  </si>
-  <si>
-    <t>[웰컴템-100원] 더캣츠 베로베로젤 닭&amp;참치 10gx20p</t>
-  </si>
-  <si>
-    <t>김효정</t>
-  </si>
-  <si>
-    <t>010-2792-5596</t>
-  </si>
-  <si>
-    <t>16959</t>
-  </si>
-  <si>
-    <t>경기도 용인시 기흥구 기흥로116번길 5 (새릉골풍림아파트) 102동 1702호</t>
-  </si>
-  <si>
-    <t>509255531201</t>
-  </si>
-  <si>
-    <t>COM4</t>
-  </si>
-  <si>
-    <t>100056849185</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:03:00</t>
-  </si>
-  <si>
-    <t>2020-10-05 오후 3:57:20</t>
-  </si>
-  <si>
-    <t>2020-10-06 오전 7:29:21</t>
-  </si>
-  <si>
-    <t>2010051556318808 394930</t>
-  </si>
-  <si>
-    <t>1000012362</t>
-  </si>
-  <si>
-    <t>앤디와 친구들 라텍스 토이</t>
-  </si>
-  <si>
-    <t>선택:데이지(닭)</t>
-  </si>
-  <si>
-    <t>이서윤</t>
-  </si>
-  <si>
-    <t>010-4224-1908</t>
-  </si>
-  <si>
-    <t>05501</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 올림픽로 99 (잠실엘스) 132-2304</t>
-  </si>
-  <si>
-    <t>509255531503</t>
   </si>
   <si>
     <t>103247553909</t>
@@ -877,13 +874,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,17 +1497,17 @@
       <c r="AP2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AQ2" s="4" t="s">
-        <v>70</v>
+      <c r="AQ2" s="4">
+        <v>7</v>
       </c>
       <c r="AR2" s="3"/>
-      <c r="AS2" s="4" t="s">
-        <v>70</v>
+      <c r="AS2" s="4">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>46</v>
@@ -1528,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>52</v>
@@ -1543,17 +1540,17 @@
         <v>54</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>59</v>
@@ -1596,52 +1593,52 @@
         <v>0</v>
       </c>
       <c r="AE3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AH3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="AO3" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>1</v>
       </c>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="4" t="s">
-        <v>84</v>
+      <c r="AS3" s="4">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>46</v>
@@ -1659,10 +1656,10 @@
         <v>50</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>52</v>
@@ -1674,17 +1671,17 @@
         <v>54</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>59</v>
@@ -1727,40 +1724,40 @@
         <v>0</v>
       </c>
       <c r="AE4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AH4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="AO4" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AQ4" s="4">
         <v>2</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>46</v>
@@ -1790,10 +1787,10 @@
         <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>52</v>
@@ -1805,17 +1802,17 @@
         <v>54</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>59</v>
@@ -1858,52 +1855,52 @@
         <v>0</v>
       </c>
       <c r="AE5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AM5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AH5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL5" s="3" t="s">
+      <c r="AN5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="AM5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN5" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="AO5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AR5" s="3"/>
       <c r="AS5" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>46</v>
@@ -1921,10 +1918,10 @@
         <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>52</v>
@@ -1936,17 +1933,17 @@
         <v>54</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>59</v>
@@ -1989,52 +1986,52 @@
         <v>0</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AM6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AN6" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="AM6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN6" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="AO6" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AR6" s="3"/>
       <c r="AS6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
@@ -2049,16 +2046,16 @@
         <v>49</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>53</v>
@@ -2067,17 +2064,17 @@
         <v>54</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>59</v>
@@ -2120,40 +2117,40 @@
         <v>0</v>
       </c>
       <c r="AE7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AF7" s="3" t="s">
+      <c r="AH7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI7" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AG7" s="3" t="s">
+      <c r="AJ7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL7" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AH7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI7" s="3" t="s">
+      <c r="AM7" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AJ7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL7" s="3" t="s">
+      <c r="AN7" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="AM7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AN7" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="AO7" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AQ7" s="4">
         <v>3</v>
@@ -2165,31 +2162,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>53</v>
@@ -2198,13 +2195,13 @@
         <v>54</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -2212,7 +2209,7 @@
         <v>59</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>59</v>
@@ -2252,69 +2249,69 @@
       </c>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM8" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="AI8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM8" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="AN8" s="3"/>
       <c r="AO8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AQ8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AR8" s="3"/>
       <c r="AS8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>53</v>
@@ -2323,13 +2320,13 @@
         <v>54</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -2337,7 +2334,7 @@
         <v>59</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>59</v>
@@ -2377,67 +2374,67 @@
       </c>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM9" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="AL9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AM9" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="AN9" s="3"/>
       <c r="AO9" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP9" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AQ9" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AR9" s="3"/>
       <c r="AS9" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>53</v>
@@ -2446,23 +2443,23 @@
         <v>54</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>59</v>
@@ -2502,67 +2499,67 @@
       </c>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AI10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM10" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="AL10" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM10" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="AN10" s="3"/>
       <c r="AO10" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP10" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AQ10" s="5" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="AR10" s="3"/>
       <c r="AS10" s="5" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>53</v>
@@ -2571,13 +2568,13 @@
         <v>54</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -2623,55 +2620,55 @@
       </c>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG11" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AG11" s="3" t="s">
+      <c r="AH11" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AH11" s="3" t="s">
+      <c r="AK11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AI11" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
+      <c r="AL11" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AK11" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL11" s="3" t="s">
+      <c r="AM11" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AM11" s="3" t="s">
+      <c r="AN11" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="AN11" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="AO11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP11" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ11" s="4">
         <v>8</v>
       </c>
       <c r="AR11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AS11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>48</v>
@@ -2680,16 +2677,16 @@
         <v>49</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>53</v>
@@ -2698,13 +2695,13 @@
         <v>54</v>
       </c>
       <c r="L12" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -2734,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="Z12" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB12" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="AC12" s="4">
         <v>0</v>
@@ -2750,67 +2747,67 @@
       </c>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG12" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="AG12" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM12" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="AM12" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="AN12" s="3"/>
       <c r="AO12" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ12" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="AQ12" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="AR12" s="3"/>
       <c r="AS12" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>53</v>
@@ -2819,17 +2816,17 @@
         <v>54</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>59</v>
@@ -2857,13 +2854,13 @@
         <v>1</v>
       </c>
       <c r="Z13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB13" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="AC13" s="4">
         <v>0</v>
@@ -2873,67 +2870,67 @@
       </c>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AJ13" s="3" t="s">
+      <c r="AK13" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AL13" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AK13" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AL13" s="3" t="s">
+      <c r="AM13" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="AM13" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="AN13" s="3"/>
       <c r="AO13" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP13" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AQ13" s="4">
         <v>9</v>
       </c>
       <c r="AR13" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AS13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>53</v>
@@ -2942,13 +2939,13 @@
         <v>54</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2994,35 +2991,35 @@
       </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG14" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AG14" s="3" t="s">
+      <c r="AH14" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="AH14" s="3" t="s">
+      <c r="AI14" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="AI14" s="3" t="s">
+      <c r="AJ14" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="AJ14" s="3" t="s">
+      <c r="AK14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL14" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="AK14" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="AL14" s="3" t="s">
+      <c r="AM14" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="AM14" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="AN14" s="3"/>
       <c r="AO14" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP14" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AQ14" s="4">
         <v>4</v>
@@ -3032,31 +3029,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>53</v>
@@ -3065,17 +3062,17 @@
         <v>54</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>59</v>
@@ -3103,14 +3100,14 @@
         <v>1</v>
       </c>
       <c r="Z15" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB15" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AA15" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="AC15" s="4">
         <v>0</v>
       </c>
@@ -3118,47 +3115,47 @@
         <v>0</v>
       </c>
       <c r="AE15" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF15" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="AF15" s="3" t="s">
+      <c r="AG15" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="AG15" s="3" t="s">
+      <c r="AH15" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AH15" s="3" t="s">
+      <c r="AI15" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL15" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="AI15" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AK15" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AL15" s="3" t="s">
+      <c r="AM15" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AM15" s="3" t="s">
+      <c r="AN15" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="AN15" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="AO15" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AP15" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AQ15" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="AQ15" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="AR15" s="3"/>
       <c r="AS15" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>